<commit_message>
1.2016-1-10 QA 2.2016-1-10 学习计划更新
</commit_message>
<xml_diff>
--- a/学习计划每日进展.xlsx
+++ b/学习计划每日进展.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>DATE</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -105,10 +105,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>项目困难，没有时间，周六晚上照例去妈妈那儿吃饭。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>时光飞逝</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -120,12 +116,32 @@
     <t>done</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>项目困难，没有时间，周六晚上照例去妈妈那儿吃饭。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>谢敏</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Web &amp; Http[4]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>看《计算机网络自顶向下》2.2-2.2.1节</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每个问题都有理解，但不清晰</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,6 +212,15 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
@@ -441,7 +466,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -457,8 +482,11 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -522,6 +550,12 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -546,22 +580,88 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="20% - 着色 2" xfId="4" builtinId="34"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="5" builtinId="8"/>
     <cellStyle name="汇总" xfId="3" builtinId="25"/>
     <cellStyle name="检查单元格" xfId="1" builtinId="23"/>
     <cellStyle name="注释" xfId="2" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -581,7 +681,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="CCE8CF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -863,60 +963,60 @@
   <dimension ref="A1:AZ68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" style="3"/>
-    <col min="2" max="2" width="16.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.25" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.75" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.5" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="46.25" style="3" customWidth="1"/>
-    <col min="6" max="6" width="13.125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="25.25" style="3" customWidth="1"/>
     <col min="7" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:52" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="26"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="28"/>
       <c r="K1" s="7"/>
     </row>
     <row r="2" spans="1:52" s="1" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="23"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="25"/>
       <c r="K2" s="7"/>
     </row>
     <row r="3" spans="1:52" s="13" customFormat="1" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
       <c r="J3" s="14"/>
       <c r="K3" s="14"/>
       <c r="L3" s="14"/>
@@ -984,7 +1084,7 @@
         <v>5</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I4" s="8"/>
       <c r="J4" s="15"/>
@@ -1050,7 +1150,7 @@
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="15"/>
@@ -1116,7 +1216,7 @@
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I6" s="5"/>
       <c r="J6" s="15"/>
@@ -1182,7 +1282,7 @@
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="15"/>
@@ -1236,20 +1336,20 @@
       <c r="B8" s="9">
         <v>42378.047766203701</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>20</v>
       </c>
       <c r="E8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="5" t="s">
-        <v>22</v>
-      </c>
       <c r="G8" s="5"/>
-      <c r="H8" s="30" t="s">
+      <c r="H8" s="22" t="s">
         <v>20</v>
       </c>
       <c r="I8" s="5"/>
@@ -1298,12 +1398,22 @@
       <c r="AZ8" s="17"/>
     </row>
     <row r="9" spans="1:52" x14ac:dyDescent="0.15">
-      <c r="A9" s="11"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
+      <c r="A9" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="9">
+        <v>42379.955937500003</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>26</v>
+      </c>
       <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+      <c r="E9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
@@ -4499,8 +4609,11 @@
     <mergeCell ref="A3:I3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C9" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>